<commit_message>
Initial push of ProjetBadir on pre_projet2 branch
</commit_message>
<xml_diff>
--- a/generated_files/tableau_imageScannee.xlsx
+++ b/generated_files/tableau_imageScannee.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tableau Extrait" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Statistiques" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OCR_Table" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,15 +29,8 @@
       <b val="1"/>
       <color rgb="00FFFFFF"/>
     </font>
-    <font>
-      <b val="1"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <b val="1"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -47,38 +39,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00366092"/>
-        <bgColor rgb="00366092"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E8F4FD"/>
-        <bgColor rgb="00E8F4FD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFF2CC"/>
-        <bgColor rgb="00FFF2CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E8F5E8"/>
-        <bgColor rgb="00E8F5E8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FCE4D6"/>
-        <bgColor rgb="00FCE4D6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F4CCCC"/>
-        <bgColor rgb="00F4CCCC"/>
+        <fgColor rgb="004F81BD"/>
+        <bgColor rgb="004F81BD"/>
       </patternFill>
     </fill>
   </fills>
@@ -100,31 +62,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -490,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,16 +443,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
     <col width="13" customWidth="1" min="3" max="3"/>
-    <col width="3" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>CodeApogée</t>
+          <t>Code Apogée</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -520,7 +464,6 @@
           <t>Prénom</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -538,7 +481,6 @@
           <t>ABDELOUAHED</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -553,20 +495,19 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>SOUFIANE</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr"/>
+          <t>SOUFINE</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>21011326</t>
+          <t>2ioii326</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>ABOU-EL KASEM</t>
+          <t>ABOU ELKASEM</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
@@ -574,605 +515,498 @@
           <t>KENZA</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>21010358</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>AHMYTTOU</t>
         </is>
       </c>
-      <c r="C5" s="3" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>AYA</t>
         </is>
       </c>
-      <c r="D5" s="3" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>21010266</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>210170266</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>AIDOUN</t>
         </is>
       </c>
-      <c r="C6" s="3" t="inlineStr">
-        <is>
-          <t>IBTISSAM</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="inlineStr"/>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>MBTISSAM</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>20001758</t>
         </is>
       </c>
-      <c r="B7" s="3" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>AL AZAMI</t>
         </is>
       </c>
-      <c r="C7" s="3" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>TAREK</t>
         </is>
       </c>
-      <c r="D7" s="3" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>21010287</t>
         </is>
       </c>
-      <c r="B8" s="4" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>ALLAM</t>
         </is>
       </c>
-      <c r="C8" s="4" t="inlineStr">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>ELARBI</t>
         </is>
       </c>
-      <c r="D8" s="4" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>21010482</t>
         </is>
       </c>
-      <c r="B9" s="4" t="inlineStr">
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>ARIB</t>
         </is>
       </c>
-      <c r="C9" s="4" t="inlineStr">
+      <c r="C9" s="2" t="inlineStr">
         <is>
           <t>AYMANE</t>
         </is>
       </c>
-      <c r="D9" s="4" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>21009157</t>
         </is>
       </c>
-      <c r="B10" s="4" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>AZZMAN</t>
         </is>
       </c>
-      <c r="C10" s="4" t="inlineStr">
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>NORELIMANE</t>
         </is>
       </c>
-      <c r="D10" s="4" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>21010356</t>
         </is>
       </c>
-      <c r="B11" s="5" t="inlineStr">
-        <is>
-          <t>AZZOoUuz</t>
-        </is>
-      </c>
-      <c r="C11" s="5" t="inlineStr">
-        <is>
-          <t>CHAIMAE</t>
-        </is>
-      </c>
-      <c r="D11" s="5" t="inlineStr"/>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>AZZOUZ</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>CHAINZAE</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="inlineStr">
-        <is>
-          <t>21010411</t>
-        </is>
-      </c>
-      <c r="B12" s="5" t="inlineStr">
-        <is>
-          <t>BEN IMRAN</t>
-        </is>
-      </c>
-      <c r="C12" s="5" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>21010477</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>BENIMRAN</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>AHLAM</t>
         </is>
       </c>
-      <c r="D12" s="5" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="inlineStr">
-        <is>
-          <t>21010476</t>
-        </is>
-      </c>
-      <c r="B13" s="5" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>21070476</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>BENCHINE</t>
         </is>
       </c>
-      <c r="C13" s="5" t="inlineStr">
-        <is>
-          <t>ABDELILAH</t>
-        </is>
-      </c>
-      <c r="D13" s="5" t="inlineStr"/>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>ABDELILAA</t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="inlineStr">
-        <is>
-          <t>22012817</t>
-        </is>
-      </c>
-      <c r="B14" s="6" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>22012877</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>BENMGUIRIDA</t>
         </is>
       </c>
-      <c r="C14" s="6" t="inlineStr">
+      <c r="C14" s="2" t="inlineStr">
         <is>
           <t>ANAS</t>
         </is>
       </c>
-      <c r="D14" s="6" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" s="6" t="inlineStr">
-        <is>
-          <t>21009110</t>
-        </is>
-      </c>
-      <c r="B15" s="6" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>21009770</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>BERKOUKT</t>
         </is>
       </c>
-      <c r="C15" s="6" t="inlineStr">
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>AMINE</t>
         </is>
       </c>
-      <c r="D15" s="6" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="inlineStr">
+      <c r="A16" s="2" t="inlineStr">
         <is>
           <t>21011779</t>
         </is>
       </c>
-      <c r="B16" s="6" t="inlineStr">
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>BIGAGANE</t>
         </is>
       </c>
-      <c r="C16" s="6" t="inlineStr">
-        <is>
-          <t>ABDELLAH</t>
-        </is>
-      </c>
-      <c r="D16" s="6" t="inlineStr"/>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>ABDELLAF</t>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="inlineStr">
+      <c r="A17" s="2" t="inlineStr">
         <is>
           <t>20011005</t>
         </is>
       </c>
-      <c r="B17" s="7" t="inlineStr">
+      <c r="B17" s="2" t="inlineStr">
         <is>
           <t>BOUHNINE</t>
         </is>
       </c>
-      <c r="C17" s="7" t="inlineStr">
+      <c r="C17" s="2" t="inlineStr">
         <is>
           <t>SAFAA</t>
         </is>
       </c>
-      <c r="D17" s="7" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="7" t="inlineStr">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>21002603</t>
         </is>
       </c>
-      <c r="B18" s="7" t="inlineStr">
+      <c r="B18" s="2" t="inlineStr">
         <is>
           <t>BOUKER</t>
         </is>
       </c>
-      <c r="C18" s="7" t="inlineStr">
+      <c r="C18" s="2" t="inlineStr">
         <is>
           <t>MOHAMMED</t>
         </is>
       </c>
-      <c r="D18" s="7" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" s="7" t="inlineStr">
+      <c r="A19" s="2" t="inlineStr">
         <is>
           <t>21010261</t>
         </is>
       </c>
-      <c r="B19" s="7" t="inlineStr">
-        <is>
-          <t>BOULERBAH</t>
-        </is>
-      </c>
-      <c r="C19" s="7" t="inlineStr">
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>BOULERBAF</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="inlineStr">
         <is>
           <t>YASSER</t>
         </is>
       </c>
-      <c r="D19" s="7" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
     </row>
     <row r="20">
-      <c r="A20" s="7" t="inlineStr">
+      <c r="A20" s="2" t="inlineStr">
         <is>
           <t>21011724</t>
         </is>
       </c>
-      <c r="B20" s="7" t="inlineStr">
+      <c r="B20" s="2" t="inlineStr">
         <is>
           <t>BOUNOUAR</t>
         </is>
       </c>
-      <c r="C20" s="7" t="inlineStr">
+      <c r="C20" s="2" t="inlineStr">
         <is>
           <t>MOHAMMED</t>
         </is>
       </c>
-      <c r="D20" s="7" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
     </row>
     <row r="21">
-      <c r="A21" s="7" t="inlineStr">
+      <c r="A21" s="2" t="inlineStr">
         <is>
           <t>21009025</t>
         </is>
       </c>
-      <c r="B21" s="7" t="inlineStr">
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>BOUSSAID</t>
         </is>
       </c>
-      <c r="C21" s="7" t="inlineStr">
+      <c r="C21" s="2" t="inlineStr">
         <is>
           <t>MERYEME</t>
         </is>
       </c>
-      <c r="D21" s="7" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" s="7" t="inlineStr">
-        <is>
-          <t>21010326</t>
-        </is>
-      </c>
-      <c r="B22" s="7" t="inlineStr">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>21070326</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
         <is>
           <t>CHAIBERRAS</t>
         </is>
       </c>
-      <c r="C22" s="7" t="inlineStr">
+      <c r="C22" s="2" t="inlineStr">
         <is>
           <t>SOUHAIL</t>
         </is>
       </c>
-      <c r="D22" s="7" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" s="7" t="inlineStr">
+      <c r="A23" s="2" t="inlineStr">
         <is>
           <t>21010299</t>
         </is>
       </c>
-      <c r="B23" s="7" t="inlineStr">
+      <c r="B23" s="2" t="inlineStr">
         <is>
           <t>CHERKI</t>
         </is>
       </c>
-      <c r="C23" s="7" t="inlineStr">
+      <c r="C23" s="2" t="inlineStr">
         <is>
           <t>HOUSSAM</t>
         </is>
       </c>
-      <c r="D23" s="7" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" s="7" t="inlineStr">
-        <is>
-          <t>21009475</t>
-        </is>
-      </c>
-      <c r="B24" s="7" t="inlineStr">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>27009475</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
         <is>
           <t>DAHBI</t>
         </is>
       </c>
-      <c r="C24" s="7" t="inlineStr">
+      <c r="C24" s="2" t="inlineStr">
         <is>
           <t>MOAD</t>
         </is>
       </c>
-      <c r="D24" s="7" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" s="7" t="inlineStr">
-        <is>
-          <t>21010439</t>
-        </is>
-      </c>
-      <c r="B25" s="7" t="inlineStr">
-        <is>
-          <t>ECHCHRIKI</t>
-        </is>
-      </c>
-      <c r="C25" s="7" t="inlineStr">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>21070439</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>ECHCHRIK</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="inlineStr">
         <is>
           <t>IMAD</t>
         </is>
       </c>
-      <c r="D25" s="7" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" s="7" t="inlineStr">
-        <is>
-          <t>21010403</t>
-        </is>
-      </c>
-      <c r="B26" s="7" t="inlineStr">
-        <is>
-          <t>EL ADNANI</t>
-        </is>
-      </c>
-      <c r="C26" s="7" t="inlineStr">
-        <is>
-          <t>EL MEHDI</t>
-        </is>
-      </c>
-      <c r="D26" s="7" t="inlineStr"/>
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>21070403</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>ELADNANI</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="inlineStr">
+        <is>
+          <t>ELmehDi</t>
+        </is>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="7" t="inlineStr">
+      <c r="A27" s="2" t="inlineStr">
         <is>
           <t>21010379</t>
         </is>
       </c>
-      <c r="B27" s="7" t="inlineStr">
+      <c r="B27" s="2" t="inlineStr">
         <is>
           <t>EL AIDI IDRISSI</t>
         </is>
       </c>
-      <c r="C27" s="7" t="inlineStr">
+      <c r="C27" s="2" t="inlineStr">
         <is>
           <t>ACHRAF</t>
         </is>
       </c>
-      <c r="D27" s="7" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" s="7" t="inlineStr">
+      <c r="A28" s="2" t="inlineStr">
         <is>
           <t>21010272</t>
         </is>
       </c>
-      <c r="B28" s="7" t="inlineStr">
-        <is>
-          <t>EL AOUAD</t>
-        </is>
-      </c>
-      <c r="C28" s="7" t="inlineStr">
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>ELAOUAD</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="inlineStr">
         <is>
           <t>OUAAIL</t>
         </is>
       </c>
-      <c r="D28" s="7" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" s="7" t="inlineStr">
-        <is>
-          <t>21010324</t>
-        </is>
-      </c>
-      <c r="B29" s="7" t="inlineStr">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>2i07o324</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
         <is>
           <t>EL BAKALI</t>
         </is>
       </c>
-      <c r="C29" s="7" t="inlineStr">
+      <c r="C29" s="2" t="inlineStr">
         <is>
           <t>MALAK</t>
         </is>
       </c>
-      <c r="D29" s="7" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" s="7" t="inlineStr">
-        <is>
-          <t>20007042</t>
-        </is>
-      </c>
-      <c r="B30" s="7" t="inlineStr">
-        <is>
-          <t>EL FERCHOUNI</t>
-        </is>
-      </c>
-      <c r="C30" s="7" t="inlineStr">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>200o7042</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>ELFERCHOUNI</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
         <is>
           <t>SOUKAYNA</t>
         </is>
       </c>
-      <c r="D30" s="7" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" s="7" t="inlineStr">
+      <c r="A31" s="2" t="inlineStr">
         <is>
           <t>21010274</t>
         </is>
       </c>
-      <c r="B31" s="7" t="inlineStr">
+      <c r="B31" s="2" t="inlineStr">
         <is>
           <t>EL GARTI</t>
         </is>
       </c>
-      <c r="C31" s="7" t="inlineStr">
+      <c r="C31" s="2" t="inlineStr">
         <is>
           <t>YASSINE</t>
         </is>
       </c>
-      <c r="D31" s="7" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" s="7" t="inlineStr">
+      <c r="A32" s="2" t="inlineStr">
         <is>
           <t>21010319</t>
         </is>
       </c>
-      <c r="B32" s="7" t="inlineStr">
+      <c r="B32" s="2" t="inlineStr">
         <is>
           <t>EL GHAZI</t>
         </is>
       </c>
-      <c r="C32" s="7" t="inlineStr">
+      <c r="C32" s="2" t="inlineStr">
         <is>
           <t>SILIA</t>
         </is>
       </c>
-      <c r="D32" s="7" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" s="7" t="inlineStr">
+      <c r="A33" s="2" t="inlineStr">
         <is>
           <t>19006658</t>
         </is>
       </c>
-      <c r="B33" s="7" t="inlineStr">
-        <is>
-          <t>EL HARIRI</t>
-        </is>
-      </c>
-      <c r="C33" s="7" t="inlineStr">
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>ELHARIRI</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="inlineStr">
         <is>
           <t>KENZA</t>
         </is>
-      </c>
-      <c r="D33" s="7" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="8" t="inlineStr">
-        <is>
-          <t>Statistiques du tableau</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="9" t="inlineStr">
-        <is>
-          <t>Nombre de lignes</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="9" t="inlineStr">
-        <is>
-          <t>Nombre de colonnes</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="9" t="inlineStr">
-        <is>
-          <t>Taille des groupes</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="9" t="inlineStr">
-        <is>
-          <t>Nombre de groupes</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>